<commit_message>
FIX: Agrega validación en el caso de parametros nulos en el archivo de configuración por filas vacías y actualiza expresión regular para detectar el nombre de los diplomas
</commit_message>
<xml_diff>
--- a/PARAMETROS_PROCESADOR_ARCHIVOS.xlsx
+++ b/PARAMETROS_PROCESADOR_ARCHIVOS.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProcesarDiplomas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GIT\Procesador_pdfs_obtener_nombres\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07D4CA3-7FE5-4BFF-B7E4-8B39B1E5940C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105B3908-7EA2-4213-A92B-5F98B62A7AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="16536" windowHeight="8712" xr2:uid="{84B4597D-7963-44B1-9587-F5775E9CC72E}"/>
+    <workbookView xWindow="-23148" yWindow="1356" windowWidth="19416" windowHeight="10296" activeTab="1" xr2:uid="{84B4597D-7963-44B1-9587-F5775E9CC72E}"/>
   </bookViews>
   <sheets>
     <sheet name="Rutas" sheetId="2" r:id="rId1"/>
     <sheet name="Documentos" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>DIPLOMA</t>
   </si>
@@ -135,10 +135,13 @@
     <t>EXCELENCIA DEL TRABAJO</t>
   </si>
   <si>
-    <t>C:/DiplomasProcesar</t>
-  </si>
-  <si>
-    <t>C:/DiplomasProcesados4-04-2024</t>
+    <t>C:\Septiembre</t>
+  </si>
+  <si>
+    <t>C:\Diplomasporprocesar</t>
+  </si>
+  <si>
+    <t>DEL\s+AÑO\s+\d{4}\.([^\n]+)</t>
   </si>
 </sst>
 </file>
@@ -569,13 +572,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925C205F-7292-4573-8DA7-A40F015494F8}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="2" width="69.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -592,7 +595,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -600,7 +603,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -617,17 +620,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D638BA71-1B96-43C1-B575-2FA6FB704DF7}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.21875" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
     <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="34.21875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" style="6" customWidth="1"/>
     <col min="4" max="6" width="55.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -653,7 +656,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -661,68 +664,73 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7" s="3"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" s="7"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="C14" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MOD: Actualización para incluir formatos de revisión de otras facultades
</commit_message>
<xml_diff>
--- a/PARAMETROS_PROCESADOR_ARCHIVOS.xlsx
+++ b/PARAMETROS_PROCESADOR_ARCHIVOS.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GIT\Procesador_pdfs_obtener_nombres\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\git\Trabajos\Procesador_pdfs_obtener_nombres\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105B3908-7EA2-4213-A92B-5F98B62A7AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433CB412-B55F-44CE-A356-A9C4BF55C476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1356" windowWidth="19416" windowHeight="10296" activeTab="1" xr2:uid="{84B4597D-7963-44B1-9587-F5775E9CC72E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{84B4597D-7963-44B1-9587-F5775E9CC72E}"/>
   </bookViews>
   <sheets>
     <sheet name="Rutas" sheetId="2" r:id="rId1"/>
     <sheet name="Documentos" sheetId="1" r:id="rId2"/>
+    <sheet name="ExpresionesXFacultad" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,9 +45,9 @@
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{FFF406F3-7AA4-4F6E-8A38-1E32FA506986}">
       <text>
-        <t>[Comentario encadenado]
-Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
-Comentario:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Permite verificar que aunque se encuentra la expresion regular, el tipo de documento si corresponde a lo que se espera</t>
       </text>
     </comment>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
   <si>
     <t>DIPLOMA</t>
   </si>
@@ -114,9 +115,6 @@
     <t>RUTA_DIRECTORIO_PROCESAR</t>
   </si>
   <si>
-    <t>RUTA_DIRECTORIO_SALIDA</t>
-  </si>
-  <si>
     <t>Mención_honor_tg</t>
   </si>
   <si>
@@ -135,20 +133,41 @@
     <t>EXCELENCIA DEL TRABAJO</t>
   </si>
   <si>
-    <t>C:\Septiembre</t>
-  </si>
-  <si>
-    <t>C:\Diplomasporprocesar</t>
-  </si>
-  <si>
     <t>DEL\s+AÑO\s+\d{4}\.([^\n]+)</t>
+  </si>
+  <si>
+    <t>DECANO DE FACULTAD([^\n]+)</t>
+  </si>
+  <si>
+    <t>([A-ZÁÉÍÓÚÑ ]{3,})\s+Quien se identifica con</t>
+  </si>
+  <si>
+    <t>EL T[ÍI]TULO\s+DE\s*([A-ZÁÉÍÓÚÑ]+(?:\s+[A-ZÁÉÍÓÚÑ]+){1,3})</t>
+  </si>
+  <si>
+    <t>DECANO DE FACULT\s*AD\s*([^\n]+)</t>
+  </si>
+  <si>
+    <t>FCSL</t>
+  </si>
+  <si>
+    <t>FHCS</t>
+  </si>
+  <si>
+    <t>FIC</t>
+  </si>
+  <si>
+    <t>FCEA</t>
+  </si>
+  <si>
+    <t>W:\ABRIL 2025 FCYH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +204,20 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF8C8C8C"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,12 +239,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -222,6 +252,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,13 +604,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925C205F-7292-4573-8DA7-A40F015494F8}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="2" width="69.88671875" customWidth="1"/>
@@ -594,23 +628,15 @@
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="B4" s="3"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="B12" s="3"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -620,116 +646,174 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D638BA71-1B96-43C1-B575-2FA6FB704DF7}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.21875" customWidth="1"/>
     <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" style="6" customWidth="1"/>
-    <col min="4" max="6" width="55.88671875" customWidth="1"/>
+    <col min="3" max="3" width="64.88671875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="55.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" customHeight="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>28</v>
+      <c r="C2" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5" ht="15.6" customHeight="1">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.8" customHeight="1">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.8" customHeight="1">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.8" customHeight="1">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -737,4 +821,106 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B292E7-25E0-4667-A68A-08C70C9A82FF}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="52.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.8" customHeight="1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>